<commit_message>
fall 2022 price change
</commit_message>
<xml_diff>
--- a/spreadsheets/pricing.xlsx
+++ b/spreadsheets/pricing.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/akr/BBP/monasmakerie/site/spreadsheets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raikh\Desktop\Aboudi\TECH\monasmakerie\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6424BE8-EC65-9D40-86F8-E72B0377888E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE47C292-4AAA-494E-BADE-955D3EAFA602}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="87">
   <si>
     <t>WAX</t>
   </si>
@@ -66,9 +66,6 @@
     <t>Bridesmaids</t>
   </si>
   <si>
-    <t>facial and peel</t>
-  </si>
-  <si>
     <t>85 each</t>
   </si>
   <si>
@@ -258,9 +255,6 @@
     <t>Bio-Élita Aqua Detox Charcoal Facial</t>
   </si>
   <si>
-    <t>A real detox and hydrating booster facial. A mask woven from cellulose and charcoal, deeply cleanses,purifies and detoxifies the skin by removing impurities, toxins and excess sebum while preserving the skins hydrolipidic film. Best for dehydrated, demanding and sensitive skins.</t>
-  </si>
-  <si>
     <t>Caviar Eye Treatment</t>
   </si>
   <si>
@@ -292,6 +286,15 @@
   </si>
   <si>
     <t>Makeup Class</t>
+  </si>
+  <si>
+    <t>A european facial with the addition of Sothys Lactic Acid Peel that resurfaces superficial lines and stimulates cell rejuvenation and brightening. Followed by a manual extraction and Mona's unique signature massage. Topping the treatment with a soothing ampule and Sothys W+ Brightening mask to complete this non-irritating acid treatment.</t>
+  </si>
+  <si>
+    <t>A real detox and hydrating booster facial. A mask woven from cellulose and charcoal, deeply cleanses,purifies and detoxifies the skin by removing impurities, toxins and excess sebum while preserving the skin's hydrolipidic film. Best for dehydrated, demanding and sensitive skin.</t>
+  </si>
+  <si>
+    <t>*NEW* Mona's Brightening Facial</t>
   </si>
 </sst>
 </file>
@@ -368,16 +371,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="10">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -600,11 +603,11 @@
   </sheetPr>
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="128" zoomScaleNormal="128" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="128" zoomScaleNormal="128" workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
@@ -620,13 +623,13 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1">
       <c r="A2" s="2"/>
       <c r="B2" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D2" s="2">
         <v>15</v>
@@ -638,7 +641,7 @@
     <row r="3" spans="1:6" ht="15.75" customHeight="1">
       <c r="A3" s="2"/>
       <c r="B3" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D3" s="2">
         <v>20</v>
@@ -650,7 +653,7 @@
     <row r="4" spans="1:6" ht="15.75" customHeight="1">
       <c r="A4" s="2"/>
       <c r="B4" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D4" s="2">
         <v>15</v>
@@ -662,7 +665,7 @@
     <row r="5" spans="1:6" ht="15.75" customHeight="1">
       <c r="A5" s="2"/>
       <c r="B5" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D5" s="2">
         <v>35</v>
@@ -674,7 +677,7 @@
     <row r="6" spans="1:6" ht="15.75" customHeight="1">
       <c r="A6" s="2"/>
       <c r="B6" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D6" s="2">
         <v>20</v>
@@ -686,7 +689,7 @@
     <row r="7" spans="1:6" ht="15.75" customHeight="1">
       <c r="A7" s="2"/>
       <c r="B7" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D7" s="2">
         <v>20</v>
@@ -698,7 +701,7 @@
     <row r="8" spans="1:6" ht="15.75" customHeight="1">
       <c r="A8" s="2"/>
       <c r="B8" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D8" s="2">
         <v>15</v>
@@ -711,7 +714,7 @@
     <row r="9" spans="1:6" ht="15.75" customHeight="1">
       <c r="A9" s="2"/>
       <c r="B9" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D9" s="2">
         <v>15</v>
@@ -724,7 +727,7 @@
     <row r="10" spans="1:6" ht="15.75" customHeight="1">
       <c r="A10" s="2"/>
       <c r="B10" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D10" s="2">
         <v>15</v>
@@ -736,7 +739,7 @@
     <row r="11" spans="1:6" ht="15.75" customHeight="1">
       <c r="A11" s="2"/>
       <c r="B11" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D11" s="2">
         <v>15</v>
@@ -748,7 +751,7 @@
     <row r="12" spans="1:6" ht="15.75" customHeight="1">
       <c r="A12" s="2"/>
       <c r="B12" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D12" s="2">
         <v>15</v>
@@ -760,7 +763,7 @@
     <row r="13" spans="1:6" ht="15.75" customHeight="1">
       <c r="A13" s="2"/>
       <c r="B13" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D13" s="2">
         <v>15</v>
@@ -772,7 +775,7 @@
     <row r="14" spans="1:6" ht="15.75" customHeight="1">
       <c r="A14" s="2"/>
       <c r="B14" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D14" s="2">
         <v>45</v>
@@ -784,7 +787,7 @@
     <row r="15" spans="1:6" ht="15.75" customHeight="1">
       <c r="A15" s="2"/>
       <c r="B15" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D15" s="2">
         <v>25</v>
@@ -796,7 +799,7 @@
     <row r="16" spans="1:6" ht="15.75" customHeight="1">
       <c r="A16" s="2"/>
       <c r="B16" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D16" s="2">
         <v>25</v>
@@ -808,7 +811,7 @@
     <row r="17" spans="1:9" ht="15.75" customHeight="1">
       <c r="A17" s="2"/>
       <c r="B17" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D17" s="2">
         <v>15</v>
@@ -820,7 +823,7 @@
     <row r="18" spans="1:9" ht="15.75" customHeight="1">
       <c r="A18" s="2"/>
       <c r="B18" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D18" s="2">
         <v>95</v>
@@ -832,7 +835,7 @@
     <row r="19" spans="1:9" ht="15.75" customHeight="1">
       <c r="A19" s="2"/>
       <c r="B19" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D19" s="2">
         <v>65</v>
@@ -844,7 +847,7 @@
     <row r="20" spans="1:9" ht="15.75" customHeight="1">
       <c r="A20" s="2"/>
       <c r="B20" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D20" s="2">
         <v>45</v>
@@ -856,7 +859,7 @@
     <row r="21" spans="1:9" ht="15.75" customHeight="1">
       <c r="A21" s="2"/>
       <c r="B21" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D21" s="2">
         <v>15</v>
@@ -868,7 +871,7 @@
     <row r="22" spans="1:9" ht="15.75" customHeight="1">
       <c r="A22" s="2"/>
       <c r="B22" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D22" s="2">
         <v>45</v>
@@ -880,7 +883,7 @@
     <row r="23" spans="1:9" ht="15.75" customHeight="1">
       <c r="A23" s="2"/>
       <c r="B23" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D23" s="2">
         <v>60</v>
@@ -892,7 +895,7 @@
     <row r="24" spans="1:9" ht="15.75" customHeight="1">
       <c r="A24" s="2"/>
       <c r="B24" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D24" s="2">
         <v>80</v>
@@ -904,7 +907,7 @@
     <row r="25" spans="1:9" ht="15.75" customHeight="1">
       <c r="A25" s="2"/>
       <c r="B25" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D25" s="2">
         <v>50</v>
@@ -916,7 +919,7 @@
     <row r="26" spans="1:9" ht="15.75" customHeight="1">
       <c r="A26" s="2"/>
       <c r="B26" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D26" s="2">
         <v>20</v>
@@ -928,7 +931,7 @@
     <row r="27" spans="1:9" ht="15.75" customHeight="1">
       <c r="A27" s="2"/>
       <c r="B27" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D27" s="2">
         <v>20</v>
@@ -940,7 +943,7 @@
     <row r="28" spans="1:9" ht="15.75" customHeight="1">
       <c r="A28" s="2"/>
       <c r="B28" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D28" s="2">
         <v>15</v>
@@ -979,13 +982,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView zoomScale="128" zoomScaleNormal="128" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" zoomScale="128" zoomScaleNormal="128" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
@@ -1001,7 +1004,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -1009,7 +1012,7 @@
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2" s="2"/>
       <c r="D2" s="2">
@@ -1019,15 +1022,15 @@
         <v>55</v>
       </c>
       <c r="F2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1">
       <c r="A3" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E3">
         <v>55</v>
@@ -1035,10 +1038,10 @@
     </row>
     <row r="4" spans="1:6" ht="15.75" customHeight="1">
       <c r="A4" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E4">
         <v>55</v>
@@ -1046,12 +1049,10 @@
     </row>
     <row r="5" spans="1:6" ht="15.75" customHeight="1">
       <c r="A5" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" s="2"/>
-      <c r="C5" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="C5" s="2"/>
       <c r="D5" s="2">
         <v>185</v>
       </c>
@@ -1059,155 +1060,171 @@
         <v>75</v>
       </c>
       <c r="F5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15.75" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>73</v>
+        <v>86</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2">
-        <v>150</v>
+        <v>195</v>
       </c>
       <c r="E6">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="F6" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2">
-        <v>180</v>
+        <v>165</v>
       </c>
       <c r="E7">
-        <v>70</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>69</v>
+        <v>60</v>
+      </c>
+      <c r="F7" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15.75" customHeight="1">
       <c r="A8" s="2" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2">
+        <v>200</v>
+      </c>
+      <c r="E8">
         <v>70</v>
       </c>
-      <c r="E8">
-        <v>30</v>
-      </c>
       <c r="F8" s="9" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15.75" customHeight="1">
       <c r="A9" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2">
-        <v>225</v>
+        <v>70</v>
       </c>
       <c r="E9">
-        <v>70</v>
+        <v>30</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15.75" customHeight="1">
       <c r="A10" s="2" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2">
-        <v>130</v>
+        <v>250</v>
       </c>
       <c r="E10">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15.75" customHeight="1">
       <c r="A11" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2">
-        <v>105</v>
+        <v>145</v>
       </c>
       <c r="E11">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15.75" customHeight="1">
       <c r="A12" s="2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="E12">
         <v>45</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15.75" customHeight="1">
       <c r="A13" s="2" t="s">
-        <v>15</v>
+        <v>76</v>
       </c>
       <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
       <c r="D13" s="2">
-        <v>75</v>
+        <v>95</v>
       </c>
       <c r="E13">
         <v>45</v>
       </c>
-      <c r="F13" t="s">
-        <v>62</v>
+      <c r="F13" s="9" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A14" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>12</v>
+      <c r="A14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="D14" s="2">
+        <v>75</v>
       </c>
       <c r="E14">
         <v>45</v>
       </c>
+      <c r="F14" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="15" spans="1:6" ht="15.75" customHeight="1">
       <c r="A15" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D15" s="2">
+        <v>53</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A16" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="2">
         <v>50</v>
       </c>
-      <c r="E15">
+      <c r="E16">
         <v>15</v>
       </c>
     </row>
@@ -1227,7 +1244,7 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" customHeight="1">
       <c r="A1" s="4" t="s">
@@ -1243,16 +1260,16 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1">
       <c r="A2" s="2"/>
       <c r="B2" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="2">
@@ -1262,13 +1279,13 @@
         <v>30</v>
       </c>
       <c r="F2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1">
       <c r="A3" s="3"/>
       <c r="B3" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="2">
@@ -1278,13 +1295,13 @@
         <v>55</v>
       </c>
       <c r="F3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" customHeight="1">
       <c r="A4" s="3"/>
       <c r="B4" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2">
@@ -1294,17 +1311,17 @@
         <v>55</v>
       </c>
       <c r="F4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15.75" customHeight="1">
       <c r="A5" s="2"/>
       <c r="B5" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E5">
         <v>55</v>
@@ -1313,7 +1330,7 @@
     <row r="6" spans="1:6" ht="15.75" customHeight="1">
       <c r="A6" s="3"/>
       <c r="B6" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2">
@@ -1323,13 +1340,13 @@
         <v>55</v>
       </c>
       <c r="F6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" customHeight="1">
       <c r="A7" s="3"/>
       <c r="B7" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2">
@@ -1339,7 +1356,7 @@
         <v>75</v>
       </c>
       <c r="F7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15.75" customHeight="1">
@@ -1362,7 +1379,7 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
@@ -1378,15 +1395,15 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" customHeight="1">
       <c r="B2" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D2" s="2">
         <v>75</v>
@@ -1397,7 +1414,7 @@
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1">
       <c r="B3" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D3" s="2">
         <v>50</v>
@@ -1408,7 +1425,7 @@
     </row>
     <row r="4" spans="1:5" ht="15.75" customHeight="1">
       <c r="B4" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D4" s="2">
         <v>25</v>
@@ -1419,7 +1436,7 @@
     </row>
     <row r="5" spans="1:5" ht="15.75" customHeight="1">
       <c r="B5" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D5" s="2">
         <v>100</v>
@@ -1430,7 +1447,7 @@
     </row>
     <row r="6" spans="1:5" ht="15.75" customHeight="1">
       <c r="B6" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D6" s="2">
         <v>300</v>
@@ -1452,7 +1469,7 @@
     </row>
     <row r="8" spans="1:5" ht="15.75" customHeight="1">
       <c r="B8" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D8" s="2">
         <v>200</v>
@@ -1472,7 +1489,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
before new menu push
</commit_message>
<xml_diff>
--- a/spreadsheets/pricing.xlsx
+++ b/spreadsheets/pricing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raiab\Stuff\TECH\monasmakerie\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1C32007-BCC1-4FB8-B94C-6EFD3D91A6E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34F11A69-C4EE-4187-90F5-B0A367E1CCB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -305,11 +305,31 @@
     <t>*NEW* Intraceuticals Oxygen Facial</t>
   </si>
   <si>
+    <t>$150 each</t>
+  </si>
+  <si>
+    <t>$85</t>
+  </si>
+  <si>
+    <t>$170</t>
+  </si>
+  <si>
+    <t>$180</t>
+  </si>
+  <si>
+    <t>$200</t>
+  </si>
+  <si>
+    <t>$250</t>
+  </si>
+  <si>
+    <t>&lt;strike style="color:red"&gt;&lt;span style="color:initial"&gt;$220&lt;/span&gt;&lt;/strike&gt; &lt;span style="color:red"&gt;$195 &lt;i&gt;until 09/15/2023&lt;/i&gt;&lt;/span&gt;</t>
+  </si>
+  <si>
     <t>Immerse yourself in the Intraceuticals Oxygen Facial, a revolutionary treatment in the professional skin care market which infuses your skin with deeply hydrating, plumping, and brightening ingredients, leaving your skin radiant, refreshed and glowing.&lt;br&gt;&lt;br&gt;
-This treatment offers a crossover which validates relaxation and pampering aspects of the service, delivering dramatic instant results, in no time.&lt;br&gt;&lt;br&gt;
-Depending on your skin type, you may select from one of the following facial options:&lt;br&gt;&lt;br&gt;
+Depending on your skin type, you may select from &lt;i&gt;one&lt;/i&gt; of the following facial options:&lt;br&gt;&lt;br&gt;
 &lt;li&gt;&lt;b&gt;Rejuvenate:&lt;/b&gt; Hydrate - Lift - Tighten&lt;/li&gt;
-&lt;li&gt;&lt;b&gt;Opulence:&lt;/b&gt; Illuminate - Brighten - Tighten&lt;/li&gt;
+&lt;li&gt;&lt;b&gt;Opulence:&lt;/b&gt; Illuminate - Brighten&lt;/li&gt;
 &lt;li&gt;&lt;b&gt;Clarity:&lt;/b&gt; Clear - Refine - Calm&lt;/li&gt;
 &lt;br&gt;
 &lt;h3  id="add-on"&gt;Professional Add-on Serums&lt;/h3&gt;
@@ -323,27 +343,6 @@
 &lt;h3 id="add-on"&gt;Professional Add-on Zoning Masks&lt;/h3&gt;
 &lt;li&gt;&lt;b&gt;Rejuvenate moisture rich eye mask &lt;b&gt;| $10&lt;/b&gt;&lt;/li&gt;
 &lt;li&gt;&lt;b&gt;Rejuvenate moisture rich lip mask &lt;b&gt;| $10&lt;/b&gt;&lt;/li&gt;</t>
-  </si>
-  <si>
-    <t>&lt;strike style="color:red"&gt;&lt;span style="color:initial"&gt;$220&lt;/span&gt;&lt;/strike&gt; &lt;span style="color:red"&gt;$195&lt;/span&gt;</t>
-  </si>
-  <si>
-    <t>$150 each</t>
-  </si>
-  <si>
-    <t>$85</t>
-  </si>
-  <si>
-    <t>$170</t>
-  </si>
-  <si>
-    <t>$180</t>
-  </si>
-  <si>
-    <t>$200</t>
-  </si>
-  <si>
-    <t>$250</t>
   </si>
 </sst>
 </file>
@@ -1337,7 +1336,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="128" zoomScaleNormal="128" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1372,13 +1371,13 @@
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="13" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="E2" s="7">
         <v>60</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1">
@@ -1388,7 +1387,7 @@
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="13" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E3">
         <v>30</v>
@@ -1404,7 +1403,7 @@
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="13" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E4">
         <v>55</v>
@@ -1420,7 +1419,7 @@
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="13" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E5">
         <v>55</v>
@@ -1436,7 +1435,7 @@
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="14" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E6">
         <v>55</v>
@@ -1449,7 +1448,7 @@
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="13" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E7">
         <v>55</v>
@@ -1465,7 +1464,7 @@
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="13" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E8">
         <v>75</v>

</xml_diff>